<commit_message>
fixed bad file path
</commit_message>
<xml_diff>
--- a/data/gc_data/excluded_gc_data.xlsx
+++ b/data/gc_data/excluded_gc_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tacaro/Documents/GitHub/Oman-2023/data/gc_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181B4FE6-2C63-A246-9471-4B229DACD7AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CD26214-F46B-884E-BE4A-ED48798749E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30260" yWindow="800" windowWidth="28040" windowHeight="17440" xr2:uid="{B592AF6A-8D5C-0349-AC49-E22236C69244}"/>
+    <workbookView xWindow="48340" yWindow="7140" windowWidth="28040" windowHeight="17440" xr2:uid="{B592AF6A-8D5C-0349-AC49-E22236C69244}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,61 +41,61 @@
     <t>excluded</t>
   </si>
   <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_05.RES</t>
-  </si>
-  <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_08.RES</t>
-  </si>
-  <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_11.RES</t>
-  </si>
-  <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_51.RES</t>
-  </si>
-  <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_14.RES</t>
-  </si>
-  <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_17.RES</t>
-  </si>
-  <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_21.RES</t>
-  </si>
-  <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_18.RES</t>
-  </si>
-  <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_20.RES</t>
-  </si>
-  <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_06.RES</t>
-  </si>
-  <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_07.RES</t>
-  </si>
-  <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_13.RES</t>
-  </si>
-  <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_12.RES</t>
-  </si>
-  <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_15.RES</t>
-  </si>
-  <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_16.RES</t>
-  </si>
-  <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_47.RES</t>
-  </si>
-  <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_50.RES</t>
-  </si>
-  <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_09.RES</t>
-  </si>
-  <si>
-    <t>data/gc_data/1jun23/01JUN23_TAC_FID_10.RES</t>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_05.RES</t>
+  </si>
+  <si>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_08.RES</t>
+  </si>
+  <si>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_11.RES</t>
+  </si>
+  <si>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_51.RES</t>
+  </si>
+  <si>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_14.RES</t>
+  </si>
+  <si>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_17.RES</t>
+  </si>
+  <si>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_21.RES</t>
+  </si>
+  <si>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_18.RES</t>
+  </si>
+  <si>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_20.RES</t>
+  </si>
+  <si>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_06.RES</t>
+  </si>
+  <si>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_07.RES</t>
+  </si>
+  <si>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_13.RES</t>
+  </si>
+  <si>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_12.RES</t>
+  </si>
+  <si>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_15.RES</t>
+  </si>
+  <si>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_16.RES</t>
+  </si>
+  <si>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_47.RES</t>
+  </si>
+  <si>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_50.RES</t>
+  </si>
+  <si>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_09.RES</t>
+  </si>
+  <si>
+    <t>data/gc_data/2023-06-01/01JUN23_TAC_FID_10.RES</t>
   </si>
 </sst>
 </file>
@@ -450,7 +450,7 @@
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>